<commit_message>
Update Document: Project Weekly Report
</commit_message>
<xml_diff>
--- a/Week 1/Project Weekly Report- VoLeThi.xlsx
+++ b/Week 1/Project Weekly Report- VoLeThi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT University\SP25\PRN222\Material\Project\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT University\SP25\PRN222\Project\PRN222\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727ADDF7-18C8-426B-8342-3641E42F44C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BD4CE3-6D4D-4B92-BA4B-4C9B879ED636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>PROJECT REPORT</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Caffeine Management</t>
   </si>
   <si>
-    <t>Khôi</t>
-  </si>
-  <si>
     <t>Hoàn thành Project plan</t>
   </si>
   <si>
@@ -145,16 +142,29 @@
   <si>
     <t>22/01/2023</t>
   </si>
+  <si>
+    <t>Hoàn thành Database Design</t>
+  </si>
+  <si>
+    <t>Đã hoàn thành thiết kế sơ bộ database và đang trong quá trình review để chốt final design</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -301,43 +311,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,7 +571,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -638,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -738,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>9</v>
@@ -747,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -776,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>9</v>
@@ -785,7 +798,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -809,20 +822,22 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>3</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>26</v>
+      <c r="B8" s="17" t="s">
+        <v>35</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>25</v>
+      <c r="C8" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="12"/>
+      <c r="E8" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1040,13 +1055,13 @@
     <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="D15" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="2"/>
@@ -1074,13 +1089,13 @@
     <row r="16" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="2"/>

</xml_diff>